<commit_message>
Sort accounts for job_budget report
</commit_message>
<xml_diff>
--- a/Job_Budget_vs_Actuals.xlsx
+++ b/Job_Budget_vs_Actuals.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37" xml:space="preserve">
   <si>
     <t>Contract Overview</t>
   </si>
@@ -17,21 +17,21 @@
     <t>Original Awarded Contract</t>
   </si>
   <si>
+    <t>Revenue Billed thru Prior Period</t>
+  </si>
+  <si>
+    <t>Change Orders</t>
+  </si>
+  <si>
+    <t>Rev Billed to Date</t>
+  </si>
+  <si>
+    <t>Total Contract Amount</t>
+  </si>
+  <si>
     <t>calc_number</t>
   </si>
   <si>
-    <t>Revenue Billed thru Prior Period</t>
-  </si>
-  <si>
-    <t>Change Orders</t>
-  </si>
-  <si>
-    <t>Rev Billed to Date</t>
-  </si>
-  <si>
-    <t>Total Contract Amount</t>
-  </si>
-  <si>
     <t>Rev this Period</t>
   </si>
   <si>
@@ -47,6 +47,9 @@
     <t>Percent Received to Date</t>
   </si>
   <si>
+    <t>calc_percent</t>
+  </si>
+  <si>
     <t>Billings in Excess of Costs</t>
   </si>
   <si>
@@ -71,52 +74,52 @@
     <t>% of Budget</t>
   </si>
   <si>
+    <t>4060 Construction Services</t>
+  </si>
+  <si>
+    <t>4065 Materials Income</t>
+  </si>
+  <si>
+    <t>5101 Wages - Direct</t>
+  </si>
+  <si>
+    <t>5102 Payroll Taxes - Direct</t>
+  </si>
+  <si>
+    <t>5501 Equipment Rental</t>
+  </si>
+  <si>
+    <t>5503 Fasteners</t>
+  </si>
+  <si>
+    <t>5505 Job Fuel</t>
+  </si>
+  <si>
+    <t>5508 Job Tools</t>
+  </si>
+  <si>
+    <t>5510 Loken Crane</t>
+  </si>
+  <si>
+    <t>5512 Safety Supplies</t>
+  </si>
+  <si>
+    <t>6000 Overhead Allocation</t>
+  </si>
+  <si>
     <t>7995 Uncategorized Expense</t>
   </si>
   <si>
-    <t>6000 Overhead Allocation</t>
-  </si>
-  <si>
-    <t>5512 Safety Supplies</t>
-  </si>
-  <si>
-    <t>5510 Loken Crane</t>
-  </si>
-  <si>
-    <t>5508 Job Tools</t>
-  </si>
-  <si>
-    <t>5505 Job Fuel</t>
-  </si>
-  <si>
-    <t>5503 Fasteners</t>
-  </si>
-  <si>
-    <t>5501 Equipment Rental</t>
-  </si>
-  <si>
-    <t>5102 Payroll Taxes - Direct</t>
-  </si>
-  <si>
-    <t>5101 Wages - Direct</t>
-  </si>
-  <si>
-    <t>4065 Materials Income</t>
-  </si>
-  <si>
-    <t>4060 Construction Services</t>
+    <t>DLH_CPT Carpenter Direct Labor Hours</t>
+  </si>
+  <si>
+    <t>DLH_FRM Foreman Direct Labor Hours</t>
+  </si>
+  <si>
+    <t>DLH_LBR Laborer Direct Labor Hours</t>
   </si>
   <si>
     <t>DLH_MR Manager Direct Labor Hours</t>
-  </si>
-  <si>
-    <t>DLH_FRM Foreman Direct Labor Hours</t>
-  </si>
-  <si>
-    <t>DLH_CPT Carpenter Direct Labor Hours</t>
-  </si>
-  <si>
-    <t>DLH_LBR Laborer Direct Labor Hours</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +169,13 @@
         <fgColor rgb="FF87B6DF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5E5F4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border/>
     <border>
       <left style="thin">
@@ -208,12 +216,17 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -227,7 +240,10 @@
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="5" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="6" numFmtId="5" fontId="0" fillId="7" applyNumberFormat="true" applyFill="true" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -329,48 +345,48 @@
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="n">
+        <v>1607012</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
+      <c r="E6" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>2</v>
+      <c r="E7" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
@@ -380,8 +396,8 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>2</v>
+      <c r="E8" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -416,7 +432,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>9</v>
@@ -435,7 +451,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
@@ -465,7 +481,7 @@
         </is>
       </c>
       <c r="C12" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
@@ -473,7 +489,7 @@
         </is>
       </c>
       <c r="E12" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -488,7 +504,7 @@
         </is>
       </c>
       <c r="C13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
@@ -496,7 +512,7 @@
         </is>
       </c>
       <c r="E13" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -507,237 +523,237 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>14</v>
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C17" s="6" t="n">
+      <c r="A17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>582835</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>279276</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>251178</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>25118</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>175000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>104895</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C28" s="0" t="n">
         <v>130910</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>104895</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>175000</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C22" s="6" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C23" s="6" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C24" s="6" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C25" s="6" t="n">
-        <v>25118</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C26" s="6" t="n">
-        <v>251178</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C27" s="6" t="n">
-        <v>279276</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C28" s="6" t="n">
-        <v>582835</v>
-      </c>
-    </row>
     <row r="29">
-      <c r="A29" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C29" s="6" t="n">
+      <c r="A29" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C30" s="6" t="n">
+      <c r="A30" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C31" s="6" t="n">
+      <c r="A31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="6" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C32" s="6" t="n">
+      <c r="A32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>